<commit_message>
EPBDS-8299 Move '[].length' deprecation check to the approprieate place
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/DeprecatedAnnotation.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/DeprecatedAnnotation.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>Step</t>
   </si>
@@ -92,6 +92,12 @@
   </si>
   <si>
     <t>java.security</t>
+  </si>
+  <si>
+    <t>arrLength</t>
+  </si>
+  <si>
+    <t>= "".bytes.length</t>
   </si>
 </sst>
 </file>
@@ -434,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:C18"/>
+  <dimension ref="B3:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,34 +539,48 @@
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C14" s="1"/>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>7</v>
-      </c>
+      <c r="C15" s="1"/>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" t="s">
-        <v>9</v>
-      </c>
+      <c r="C16" s="1"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" t="s">
-        <v>12</v>
-      </c>
+      <c r="C17" s="1"/>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>8</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>